<commit_message>
Update to deal with issue of SAE reporting where there are hard outcomes among the study endpoints
</commit_message>
<xml_diff>
--- a/Data/sae_extraction_20200131.xlsx
+++ b/Data/sae_extraction_20200131.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dvdmc\OneDrive - University of Glasgow\Documents\adverse_events_older_people\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="69" documentId="8_{10912F58-3D18-4B01-919C-DC4A349BCDFA}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{B212F1FB-FEF4-4F1E-8482-28F56BF82A3D}"/>
+  <xr:revisionPtr revIDLastSave="73" documentId="8_{10912F58-3D18-4B01-919C-DC4A349BCDFA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{8CA8DA64-17E3-48A6-88F5-960798BD11B3}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="819" activeTab="3" xr2:uid="{3137E817-FA1E-4743-A1DF-4AF79B93904D}"/>
   </bookViews>
@@ -19,7 +19,7 @@
     <sheet name="results_extract" sheetId="3" r:id="rId4"/>
     <sheet name="arm_info" sheetId="1" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +27,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -3955,9 +3957,6 @@
     <t>NA. This trial is about metformin - ?should be excluded</t>
   </si>
   <si>
-    <t>5 (0.3)</t>
-  </si>
-  <si>
     <t>1955</t>
   </si>
   <si>
@@ -3977,6 +3976,9 @@
   </si>
   <si>
     <t>DM took from paper 26996246</t>
+  </si>
+  <si>
+    <t>94 ()</t>
   </si>
 </sst>
 </file>
@@ -4637,8 +4639,8 @@
   <dimension ref="A1:I739"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A132" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B159" sqref="B159"/>
+      <pane ySplit="1" topLeftCell="A129" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B159" sqref="B159:D159"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" x14ac:dyDescent="0.35"/>
@@ -7707,7 +7709,7 @@
         <v>52</v>
       </c>
       <c r="E156" s="7" t="s">
-        <v>1307</v>
+        <v>1306</v>
       </c>
       <c r="F156" t="s">
         <v>221</v>
@@ -7727,7 +7729,7 @@
         <v>408</v>
       </c>
       <c r="E157" s="7" t="s">
-        <v>1308</v>
+        <v>1307</v>
       </c>
       <c r="F157" t="s">
         <v>221</v>
@@ -7747,7 +7749,7 @@
         <v>408</v>
       </c>
       <c r="E158" s="7" t="s">
-        <v>1309</v>
+        <v>1308</v>
       </c>
       <c r="F158" t="s">
         <v>221</v>
@@ -7767,7 +7769,7 @@
         <v>96</v>
       </c>
       <c r="E159" s="7" t="s">
-        <v>1310</v>
+        <v>1309</v>
       </c>
       <c r="F159" t="s">
         <v>221</v>
@@ -19232,7 +19234,7 @@
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C44" sqref="C44"/>
+      <selection pane="bottomLeft" activeCell="A44" sqref="A44:XFD44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" x14ac:dyDescent="0.35"/>
@@ -21057,8 +21059,8 @@
   <dimension ref="A1:J231"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A185" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H194" sqref="H194"/>
+      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E51" sqref="E51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" x14ac:dyDescent="0.35"/>
@@ -21121,10 +21123,10 @@
         <v>53</v>
       </c>
       <c r="G2" t="s">
+        <v>1310</v>
+      </c>
+      <c r="H2" t="s">
         <v>1311</v>
-      </c>
-      <c r="H2" t="s">
-        <v>1312</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
@@ -21147,7 +21149,7 @@
         <v>53</v>
       </c>
       <c r="G3" t="s">
-        <v>1311</v>
+        <v>1310</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.35">
@@ -22185,7 +22187,7 @@
         <v>582</v>
       </c>
       <c r="E51" t="s">
-        <v>1306</v>
+        <v>1313</v>
       </c>
       <c r="G51" t="s">
         <v>1010</v>
@@ -25209,7 +25211,7 @@
         <v>930</v>
       </c>
       <c r="H189" t="s">
-        <v>1313</v>
+        <v>1312</v>
       </c>
     </row>
     <row r="190" spans="1:9" x14ac:dyDescent="0.35">
@@ -25232,7 +25234,7 @@
         <v>930</v>
       </c>
       <c r="H190" t="s">
-        <v>1313</v>
+        <v>1312</v>
       </c>
     </row>
     <row r="191" spans="1:9" x14ac:dyDescent="0.35">
@@ -25255,7 +25257,7 @@
         <v>930</v>
       </c>
       <c r="H191" t="s">
-        <v>1313</v>
+        <v>1312</v>
       </c>
     </row>
     <row r="192" spans="1:9" x14ac:dyDescent="0.35">
@@ -25278,7 +25280,7 @@
         <v>930</v>
       </c>
       <c r="H192" t="s">
-        <v>1313</v>
+        <v>1312</v>
       </c>
     </row>
     <row r="193" spans="1:10" x14ac:dyDescent="0.35">
@@ -25301,7 +25303,7 @@
         <v>930</v>
       </c>
       <c r="H193" t="s">
-        <v>1313</v>
+        <v>1312</v>
       </c>
     </row>
     <row r="194" spans="1:10" x14ac:dyDescent="0.35">
@@ -25324,7 +25326,7 @@
         <v>930</v>
       </c>
       <c r="H194" t="s">
-        <v>1313</v>
+        <v>1312</v>
       </c>
     </row>
     <row r="195" spans="1:10" x14ac:dyDescent="0.35">
@@ -32623,6 +32625,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100CF7793DA0DEC7646B4067AE33236EE6A" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="39182d8c501db2feff8a634ef4fcbc54">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="c55d3ce8-937e-4dcf-883e-347e1ce052b7" xmlns:ns4="e63c1461-d352-4ca9-95af-d03a8e9eb2cb" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7e66070fc1ae4f41c651eea051476ae7" ns3:_="" ns4:_="">
     <xsd:import namespace="c55d3ce8-937e-4dcf-883e-347e1ce052b7"/>
@@ -32839,15 +32850,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -32855,6 +32857,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AC3B6662-E37F-4F37-86DF-BC6ACEE62A41}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{18578C76-3020-46A6-B114-6BEC29578938}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -32869,14 +32879,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AC3B6662-E37F-4F37-86DF-BC6ACEE62A41}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>